<commit_message>
Added some extra info to the excel export of project allocations
</commit_message>
<xml_diff>
--- a/projects2/storage/exports/ProjectAllocations.xlsx
+++ b/projects2/storage/exports/ProjectAllocations.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr date1904="1" codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>Title</t>
   </si>
@@ -32,22 +32,22 @@
     <t>1st round choices</t>
   </si>
   <si>
-    <t>Rresult</t>
+    <t>Result</t>
   </si>
   <si>
     <t>2nd round choices</t>
   </si>
   <si>
-    <t>Result</t>
-  </si>
-  <si>
     <t>Student</t>
   </si>
   <si>
-    <t xml:space="preserve"> cvbncbnvbn</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> William Allan</t>
+    <t>Allocated?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eum aut aperiam</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kathlyn Kub</t>
   </si>
   <si>
     <t>N/A</t>
@@ -59,25 +59,19 @@
     <t>Y</t>
   </si>
   <si>
-    <t>NAMEFORE2 NAMESUR2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> dbcvbcvbcv</t>
-  </si>
-  <si>
-    <t>Jenny Smith</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> dfvfdv</t>
+    <t>Glenda Gutkowski (4906013)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> non labore et</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zion Sauer</t>
   </si>
   <si>
     <t xml:space="preserve">Y </t>
   </si>
   <si>
-    <t>FORENAME1 SURNAME1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sdfdfgdfg</t>
+    <t>Addison Gutmann (3530485)</t>
   </si>
 </sst>
 </file>
@@ -441,26 +435,27 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.996582" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="17.567139" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="19.995117" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="15.281982" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="13.85376" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="16.567383" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="22.851563" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="9.997559000000001" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="8.712158000000001" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="22.851563" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="8.712158000000001" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="22.280273" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="31.706543" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="12.854004" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,13 +478,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -517,19 +515,22 @@
       <c r="I2" t="s">
         <v>14</v>
       </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -544,64 +545,11 @@
         <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="J3" t="s">
         <v>13</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -610,10 +558,6 @@
     <hyperlink ref="B2" r:id="rId_hyperlink_2"/>
     <hyperlink ref="A3" r:id="rId_hyperlink_3"/>
     <hyperlink ref="B3" r:id="rId_hyperlink_4"/>
-    <hyperlink ref="A4" r:id="rId_hyperlink_5"/>
-    <hyperlink ref="B4" r:id="rId_hyperlink_6"/>
-    <hyperlink ref="A5" r:id="rId_hyperlink_7"/>
-    <hyperlink ref="B5" r:id="rId_hyperlink_8"/>
   </hyperlinks>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="" right="" top="" bottom="" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Lots of changes that I believe I have completed but we will see.
</commit_message>
<xml_diff>
--- a/projects2/storage/exports/ProjectAllocations.xlsx
+++ b/projects2/storage/exports/ProjectAllocations.xlsx
@@ -15,60 +15,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Preallocated?</t>
-  </si>
-  <si>
-    <t>1st Round</t>
-  </si>
-  <si>
-    <t>2nd Round</t>
-  </si>
-  <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>Supervisor</t>
-  </si>
-  <si>
-    <t>Discipline</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Eugene Keeling (1650331d)</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>cumque doloremque odit</t>
-  </si>
-  <si>
-    <t>Bridget Langworth</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mohammad Steuber (4447958u)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Karson Wisozk (7512586t)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y </t>
-  </si>
-  <si>
-    <t>est porro modi (Pre)</t>
-  </si>
-  <si>
-    <t>Vivianne Rippin</t>
+    <t>University</t>
+  </si>
+  <si>
+    <t>Projects</t>
+  </si>
+  <si>
+    <t>Applied</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Jose Brown</t>
+  </si>
+  <si>
+    <t>UoG</t>
+  </si>
+  <si>
+    <t>Darion Considine</t>
+  </si>
+  <si>
+    <t>Penelope Nienow</t>
+  </si>
+  <si>
+    <t>Judy Parker</t>
   </si>
 </sst>
 </file>
@@ -76,7 +52,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -93,15 +69,6 @@
       <u val="none"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -122,14 +89,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -432,24 +396,22 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="34.134521" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="17.709961" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="12.568359" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="12.568359" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="26.993408" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="21.137695" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="13.85376" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="19.995117" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="13.85376" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="11.425781" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="9.997559000000001" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="11.425781" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,83 +427,77 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId_hyperlink_1"/>
-    <hyperlink ref="A3" r:id="rId_hyperlink_2"/>
-    <hyperlink ref="A4" r:id="rId_hyperlink_3"/>
-  </hyperlinks>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="" right="" top="" bottom="" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>

</xml_diff>

<commit_message>
Additional features added including importing spreadsheet for allocations, removing ability for staff to choose a student for their project, importing external staff will send them an email to set their password.
</commit_message>
<xml_diff>
--- a/projects2/storage/exports/ProjectAllocations.xlsx
+++ b/projects2/storage/exports/ProjectAllocations.xlsx
@@ -32,19 +32,19 @@
     <t>Accepted</t>
   </si>
   <si>
-    <t>Jose Brown</t>
+    <t>Thomas Feil</t>
   </si>
   <si>
     <t>UoG</t>
   </si>
   <si>
-    <t>Darion Considine</t>
-  </si>
-  <si>
-    <t>Penelope Nienow</t>
-  </si>
-  <si>
-    <t>Judy Parker</t>
+    <t>Tyrel Fritsch</t>
+  </si>
+  <si>
+    <t>Shaun Mraz</t>
+  </si>
+  <si>
+    <t>Rodger Weissnat</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19.995117" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="18.709717" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="13.85376" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="11.425781" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="9.997559000000001" bestFit="true" customWidth="true" style="0"/>

</xml_diff>

<commit_message>
Fixed issue with popularity bar
</commit_message>
<xml_diff>
--- a/projects2/storage/exports/ProjectAllocations.xlsx
+++ b/projects2/storage/exports/ProjectAllocations.xlsx
@@ -32,19 +32,19 @@
     <t>Accepted</t>
   </si>
   <si>
-    <t>Thomas Feil</t>
+    <t>Assunta Feil</t>
   </si>
   <si>
     <t>UoG</t>
   </si>
   <si>
-    <t>Tyrel Fritsch</t>
-  </si>
-  <si>
-    <t>Shaun Mraz</t>
-  </si>
-  <si>
-    <t>Rodger Weissnat</t>
+    <t>Al Greenholt</t>
+  </si>
+  <si>
+    <t>Keven Mueller</t>
+  </si>
+  <si>
+    <t>Katharina Shields</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="18.709717" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="21.137695" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="13.85376" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="11.425781" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="9.997559000000001" bestFit="true" customWidth="true" style="0"/>
@@ -453,13 +453,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -487,13 +487,13 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Students are not allowed to choose two projects that have the same supervisor. Have implemented this check once they submit
</commit_message>
<xml_diff>
--- a/projects2/storage/exports/ProjectAllocations.xlsx
+++ b/projects2/storage/exports/ProjectAllocations.xlsx
@@ -32,19 +32,19 @@
     <t>Accepted</t>
   </si>
   <si>
-    <t>Assunta Feil</t>
+    <t>Cloyd Goldner</t>
   </si>
   <si>
     <t>UoG</t>
   </si>
   <si>
-    <t>Al Greenholt</t>
-  </si>
-  <si>
-    <t>Keven Mueller</t>
-  </si>
-  <si>
-    <t>Katharina Shields</t>
+    <t>Gregg Grant</t>
+  </si>
+  <si>
+    <t>Destinee Orn</t>
+  </si>
+  <si>
+    <t>Alva Purdy</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="21.137695" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="13.85376" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="11.425781" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="9.997559000000001" bestFit="true" customWidth="true" style="0"/>
@@ -436,13 +436,13 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -470,13 +470,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5">

</xml_diff>

<commit_message>
Forgot to update the update method for project controller
</commit_message>
<xml_diff>
--- a/projects2/storage/exports/ProjectAllocations.xlsx
+++ b/projects2/storage/exports/ProjectAllocations.xlsx
@@ -32,19 +32,19 @@
     <t>Accepted</t>
   </si>
   <si>
-    <t>Dahlia Berge</t>
+    <t>Audreanne Adams</t>
   </si>
   <si>
     <t>UoG</t>
   </si>
   <si>
-    <t>Richie Morar</t>
-  </si>
-  <si>
-    <t>Kaleigh O-Connell</t>
-  </si>
-  <si>
-    <t>Krystal Schultz</t>
+    <t>Will Mayer</t>
+  </si>
+  <si>
+    <t>Elvie Stanton</t>
+  </si>
+  <si>
+    <t>Calista Swaniawski</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="21.137695" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="22.280273" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="13.85376" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="11.425781" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="9.997559000000001" bestFit="true" customWidth="true" style="0"/>
@@ -470,13 +470,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -487,13 +487,13 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>